<commit_message>
VestibularVR H1BOM updates & Lick Sensor step on
- VestibularVR H1
. component ref updated
. BOM file updated

- Lick Sensor module v1.0
. still only on schematic design
</commit_message>
<xml_diff>
--- a/_pcb/VestibularVR H1-module v1.0/VestibularVR H1-module v1.0 BOM.xlsx
+++ b/_pcb/VestibularVR H1-module v1.0/VestibularVR H1-module v1.0 BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David Palma\Documents\GitHub\vestibular-vr\_pcb\VestibularVR H1-module v1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AC205E-7889-4BFA-9480-C8C6DAB65A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85378EB7-5451-44EB-B8E7-DD827B542156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="513" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VestibularVR H1-module v1.0" sheetId="15" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="177">
   <si>
     <t>Qty</t>
   </si>
@@ -606,6 +606,9 @@
   </si>
   <si>
     <t>CAM_TRIGGERS, REWARD_VALVES</t>
+  </si>
+  <si>
+    <t>74VHC1GT126DT1G</t>
   </si>
 </sst>
 </file>
@@ -806,127 +809,6 @@
   </cellStyles>
   <dxfs count="34">
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1045,6 +927,127 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1237,37 +1240,37 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AC7792F2-EC84-430C-A79F-EA1B2BD96665}" name="VestibularVR_H1_module_v1_0__106" displayName="VestibularVR_H1_module_v1_0__106" ref="A5:H31" tableType="queryTable" totalsRowShown="0" headerRowDxfId="9" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AC7792F2-EC84-430C-A79F-EA1B2BD96665}" name="VestibularVR_H1_module_v1_0__106" displayName="VestibularVR_H1_module_v1_0__106" ref="A5:H31" tableType="queryTable" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A5:H31" xr:uid="{AC7792F2-EC84-430C-A79F-EA1B2BD96665}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:H31">
-    <sortCondition ref="B5:B31"/>
+    <sortCondition ref="D5:D31"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{2B44AE86-C105-4DFB-96CE-B782D59E6333}" uniqueName="1" name="Qty" queryTableFieldId="1" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{08912D9C-3405-4930-9A2A-DBEEDAACFBB9}" uniqueName="5" name="Parts" queryTableFieldId="5" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{493D5CA6-F12F-4B0E-AD37-C0F1F623607A}" uniqueName="2" name="Value" queryTableFieldId="2" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{DE635DF0-74FE-4F65-985E-4AD64518B760}" uniqueName="17" name="OEPS" queryTableFieldId="17" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{4C11DC8A-8A8A-47D0-94E9-17ACBE45BD49}" uniqueName="13" name="MPN" queryTableFieldId="13" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{CE65B4C1-3742-4C8E-9265-C4DE2528B2AD}" uniqueName="3" name="Device" queryTableFieldId="3" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{81B1A0B2-33E1-4DDF-98AB-75639FD996FA}" uniqueName="4" name="Package" queryTableFieldId="4" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{D5E7F07C-3C03-41D8-AFAA-120B17EA2027}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{2B44AE86-C105-4DFB-96CE-B782D59E6333}" uniqueName="1" name="Qty" queryTableFieldId="1" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{08912D9C-3405-4930-9A2A-DBEEDAACFBB9}" uniqueName="5" name="Parts" queryTableFieldId="5" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{493D5CA6-F12F-4B0E-AD37-C0F1F623607A}" uniqueName="2" name="Value" queryTableFieldId="2" dataDxfId="17"/>
+    <tableColumn id="17" xr3:uid="{DE635DF0-74FE-4F65-985E-4AD64518B760}" uniqueName="17" name="OEPS" queryTableFieldId="17" dataDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{4C11DC8A-8A8A-47D0-94E9-17ACBE45BD49}" uniqueName="13" name="MPN" queryTableFieldId="13" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{CE65B4C1-3742-4C8E-9265-C4DE2528B2AD}" uniqueName="3" name="Device" queryTableFieldId="3" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{81B1A0B2-33E1-4DDF-98AB-75639FD996FA}" uniqueName="4" name="Package" queryTableFieldId="4" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{D5E7F07C-3C03-41D8-AFAA-120B17EA2027}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5DD54FB0-C92C-401F-9917-C2297C33E494}" name="Table389" displayName="Table389" ref="A4:H9" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5DD54FB0-C92C-401F-9917-C2297C33E494}" name="Table389" displayName="Table389" ref="A4:H9" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
   <autoFilter ref="A4:H9" xr:uid="{5DD54FB0-C92C-401F-9917-C2297C33E494}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{1FA2FA6C-EF5A-464F-B3A6-E30158BC018E}" name="Qty" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{71B61DC8-D94F-4867-AB39-09448AFE1A27}" name="Value" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{0A060C1D-A2C0-4049-923B-973E7315F832}" name="Parts" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{BB5B70C1-A9E9-46DB-8F6D-1534F59C0CAB}" name="OEPS" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{56747753-F2BF-45BC-81ED-B4B1B7C18231}" name="Device" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{2FF7059F-FE7F-42D0-AA0F-4189E7EB0421}" name="MPN" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{25D90C52-52B1-4B93-B093-5634C21AE70D}" name="Package" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{21E1EBD7-CD9E-4CDC-888E-9EBAC2BF580B}" name="Description" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{1FA2FA6C-EF5A-464F-B3A6-E30158BC018E}" name="Qty" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{71B61DC8-D94F-4867-AB39-09448AFE1A27}" name="Value" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{0A060C1D-A2C0-4049-923B-973E7315F832}" name="Parts" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{BB5B70C1-A9E9-46DB-8F6D-1534F59C0CAB}" name="OEPS" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{56747753-F2BF-45BC-81ED-B4B1B7C18231}" name="Device" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{2FF7059F-FE7F-42D0-AA0F-4189E7EB0421}" name="MPN" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{25D90C52-52B1-4B93-B093-5634C21AE70D}" name="Package" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{21E1EBD7-CD9E-4CDC-888E-9EBAC2BF580B}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1572,15 +1575,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B330320-CBD7-4379-B9CE-E3B1A8E4AEDB}">
   <dimension ref="A2:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" customWidth="1"/>
     <col min="4" max="4" width="19.21875" customWidth="1"/>
     <col min="5" max="5" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.109375" customWidth="1"/>
@@ -1651,68 +1654,68 @@
         <v>2</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>37</v>
+        <v>97</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
+        <v>2</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
         <v>1</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B8" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C8" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D8" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E8" s="23" t="s">
         <v>107</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
-        <v>14</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>21</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>19</v>
@@ -1724,21 +1727,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>19</v>
@@ -1752,10 +1755,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="23" t="s">
         <v>33</v>
@@ -1767,39 +1770,39 @@
         <v>37</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>130</v>
+        <v>34</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>131</v>
+        <v>35</v>
       </c>
       <c r="H10" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>175</v>
+        <v>38</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>153</v>
+        <v>33</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>162</v>
+        <v>105</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>161</v>
+        <v>37</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>29</v>
+        <v>130</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>29</v>
+        <v>131</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1807,51 +1810,51 @@
         <v>2</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>72</v>
+        <v>129</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="H13" s="23" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1859,25 +1862,25 @@
         <v>4</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>50</v>
+        <v>174</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>163</v>
+        <v>23</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="H14" s="23" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1885,103 +1888,103 @@
         <v>1</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="H15" s="23" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>91</v>
+        <v>63</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="H16" s="23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="9">
         <v>1</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>60</v>
+        <v>121</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="H17" s="23" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>44</v>
+        <v>89</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>40</v>
+        <v>89</v>
       </c>
       <c r="G18" s="23" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="H18" s="23" t="s">
-        <v>43</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1989,77 +1992,77 @@
         <v>2</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>158</v>
+        <v>39</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>159</v>
+        <v>44</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>125</v>
+        <v>66</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="H20" s="23" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="G21" s="23" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H21" s="23" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -2067,25 +2070,25 @@
         <v>1</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="G22" s="23" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -2093,207 +2096,207 @@
         <v>2</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>103</v>
+        <v>27</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>97</v>
+        <v>158</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>97</v>
+        <v>160</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>97</v>
+        <v>159</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>129</v>
+        <v>175</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>24</v>
+        <v>153</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>119</v>
+        <v>162</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>25</v>
+        <v>161</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="G24" s="23" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="H24" s="23" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>174</v>
+        <v>8</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>23</v>
+        <v>165</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G25" s="23" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H25" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="9">
         <v>1</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>121</v>
+        <v>60</v>
       </c>
       <c r="F26" s="23" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="G26" s="23" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="H26" s="23" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>78</v>
+        <v>45</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>138</v>
+        <v>47</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="G27" s="23" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="H27" s="23" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="G28" s="23" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="H28" s="23" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G29" s="23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H29" s="23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>104</v>
+        <v>176</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="G30" s="23" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="H30" s="23" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -2301,25 +2304,25 @@
         <v>1</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F31" s="23" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="G31" s="23" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="H31" s="23" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="18" x14ac:dyDescent="0.35">

</xml_diff>